<commit_message>
Modified Manual Testing Project
</commit_message>
<xml_diff>
--- a/ManualTestingProject.xlsx
+++ b/ManualTestingProject.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="3"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="8" r:id="rId2"/>
     <sheet name="Test Execution" sheetId="2" r:id="rId3"/>
     <sheet name="Bug Report" sheetId="9" r:id="rId4"/>
-    <sheet name="RTM" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="2">'Test Execution'!$H$9</definedName>
@@ -2435,7 +2434,7 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
@@ -6599,7 +6598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -6724,21 +6723,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>